<commit_message>
V76 avance del 80%
</commit_message>
<xml_diff>
--- a/Distribución.xlsx
+++ b/Distribución.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2020\desarrollo web\projects comun\projectDjango\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6418FC98-10A3-442B-B733-877A4A5FD9C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBCA2EB-140F-4127-A30B-0F9BCA95AC8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D8DF3AF1-A4AA-47C3-B201-C40AAFFBA999}"/>
   </bookViews>
@@ -604,8 +604,8 @@
   <dimension ref="A1:L97"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D63" sqref="D63"/>
+      <pane ySplit="2" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G84" sqref="G84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -650,7 +650,7 @@
       </c>
       <c r="E2" s="7">
         <f>ROUND(SUM(Tabla1[Avance])*100/9500,2)/100</f>
-        <v>0.64209999999999989</v>
+        <v>0.8</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
@@ -1525,9 +1525,11 @@
         <v>2</v>
       </c>
       <c r="C64" s="2">
-        <v>0</v>
-      </c>
-      <c r="D64" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="D64" s="5">
+        <v>44116</v>
+      </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
@@ -1537,9 +1539,11 @@
         <v>2</v>
       </c>
       <c r="C65" s="2">
-        <v>0</v>
-      </c>
-      <c r="D65" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="D65" s="5">
+        <v>44117</v>
+      </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
@@ -1549,9 +1553,11 @@
         <v>2</v>
       </c>
       <c r="C66" s="2">
-        <v>0</v>
-      </c>
-      <c r="D66" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="D66" s="5">
+        <v>44117</v>
+      </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
@@ -1561,9 +1567,11 @@
         <v>2</v>
       </c>
       <c r="C67" s="2">
-        <v>0</v>
-      </c>
-      <c r="D67" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="D67" s="5">
+        <v>44117</v>
+      </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
@@ -1573,9 +1581,11 @@
         <v>2</v>
       </c>
       <c r="C68" s="2">
-        <v>0</v>
-      </c>
-      <c r="D68" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="D68" s="5">
+        <v>44118</v>
+      </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
@@ -1585,9 +1595,11 @@
         <v>2</v>
       </c>
       <c r="C69" s="2">
-        <v>0</v>
-      </c>
-      <c r="D69" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="D69" s="5">
+        <v>44118</v>
+      </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
@@ -1597,9 +1609,11 @@
         <v>2</v>
       </c>
       <c r="C70" s="2">
-        <v>0</v>
-      </c>
-      <c r="D70" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="D70" s="5">
+        <v>44118</v>
+      </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
@@ -1609,9 +1623,11 @@
         <v>2</v>
       </c>
       <c r="C71" s="2">
-        <v>0</v>
-      </c>
-      <c r="D71" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="D71" s="5">
+        <v>44121</v>
+      </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
@@ -1621,9 +1637,11 @@
         <v>2</v>
       </c>
       <c r="C72" s="2">
-        <v>0</v>
-      </c>
-      <c r="D72" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="D72" s="5">
+        <v>44121</v>
+      </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
@@ -1633,9 +1651,11 @@
         <v>3</v>
       </c>
       <c r="C73" s="2">
-        <v>0</v>
-      </c>
-      <c r="D73" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="D73" s="5">
+        <v>44123</v>
+      </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
@@ -1645,9 +1665,11 @@
         <v>3</v>
       </c>
       <c r="C74" s="2">
-        <v>0</v>
-      </c>
-      <c r="D74" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="D74" s="5">
+        <v>44123</v>
+      </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
@@ -1657,9 +1679,11 @@
         <v>3</v>
       </c>
       <c r="C75" s="2">
-        <v>0</v>
-      </c>
-      <c r="D75" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="D75" s="5">
+        <v>44123</v>
+      </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
@@ -1669,9 +1693,11 @@
         <v>3</v>
       </c>
       <c r="C76" s="2">
-        <v>0</v>
-      </c>
-      <c r="D76" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="D76" s="5">
+        <v>44124</v>
+      </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
@@ -1681,9 +1707,11 @@
         <v>3</v>
       </c>
       <c r="C77" s="2">
-        <v>0</v>
-      </c>
-      <c r="D77" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="D77" s="5">
+        <v>44124</v>
+      </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
@@ -1693,9 +1721,11 @@
         <v>3</v>
       </c>
       <c r="C78" s="2">
-        <v>0</v>
-      </c>
-      <c r="D78" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="D78" s="5">
+        <v>44124</v>
+      </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="1">

</xml_diff>

<commit_message>
V90 95% de avance
</commit_message>
<xml_diff>
--- a/Distribución.xlsx
+++ b/Distribución.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2020\desarrollo web\projects comun\projectDjango\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBCA2EB-140F-4127-A30B-0F9BCA95AC8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A71CC19-12A5-41FF-BCFD-CF128D3C5F37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D8DF3AF1-A4AA-47C3-B201-C40AAFFBA999}"/>
   </bookViews>
@@ -605,7 +605,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G84" sqref="G84"/>
+      <selection pane="bottomLeft" activeCell="G92" sqref="G92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -650,7 +650,7 @@
       </c>
       <c r="E2" s="7">
         <f>ROUND(SUM(Tabla1[Avance])*100/9500,2)/100</f>
-        <v>0.8</v>
+        <v>0.94739999999999991</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
@@ -1735,9 +1735,11 @@
         <v>3</v>
       </c>
       <c r="C79" s="2">
-        <v>0</v>
-      </c>
-      <c r="D79" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="D79" s="5">
+        <v>44125</v>
+      </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
@@ -1747,11 +1749,13 @@
         <v>3</v>
       </c>
       <c r="C80" s="2">
-        <v>0</v>
-      </c>
-      <c r="D80" s="1"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="D80" s="5">
+        <v>44125</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -1759,11 +1763,13 @@
         <v>3</v>
       </c>
       <c r="C81" s="2">
-        <v>0</v>
-      </c>
-      <c r="D81" s="1"/>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="D81" s="5">
+        <v>44125</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -1771,11 +1777,13 @@
         <v>3</v>
       </c>
       <c r="C82" s="2">
-        <v>0</v>
-      </c>
-      <c r="D82" s="1"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="D82" s="5">
+        <v>44126</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -1783,11 +1791,13 @@
         <v>2</v>
       </c>
       <c r="C83" s="2">
-        <v>0</v>
-      </c>
-      <c r="D83" s="1"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="D83" s="5">
+        <v>44126</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -1795,11 +1805,13 @@
         <v>2</v>
       </c>
       <c r="C84" s="2">
-        <v>0</v>
-      </c>
-      <c r="D84" s="1"/>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="D84" s="5">
+        <v>44126</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -1807,11 +1819,13 @@
         <v>2</v>
       </c>
       <c r="C85" s="2">
-        <v>0</v>
-      </c>
-      <c r="D85" s="1"/>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="D85" s="5">
+        <v>44126</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -1819,11 +1833,13 @@
         <v>2</v>
       </c>
       <c r="C86" s="2">
-        <v>0</v>
-      </c>
-      <c r="D86" s="1"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="D86" s="5">
+        <v>44127</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -1831,11 +1847,13 @@
         <v>2</v>
       </c>
       <c r="C87" s="2">
-        <v>0</v>
-      </c>
-      <c r="D87" s="1"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="D87" s="5">
+        <v>44127</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -1843,11 +1861,13 @@
         <v>2</v>
       </c>
       <c r="C88" s="2">
-        <v>0</v>
-      </c>
-      <c r="D88" s="1"/>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="D88" s="5">
+        <v>44127</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -1855,11 +1875,13 @@
         <v>2</v>
       </c>
       <c r="C89" s="2">
-        <v>0</v>
-      </c>
-      <c r="D89" s="1"/>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="D89" s="5">
+        <v>44128</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -1867,11 +1889,13 @@
         <v>2</v>
       </c>
       <c r="C90" s="2">
-        <v>0</v>
-      </c>
-      <c r="D90" s="1"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="D90" s="5">
+        <v>44128</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -1879,11 +1903,13 @@
         <v>2</v>
       </c>
       <c r="C91" s="2">
-        <v>0</v>
-      </c>
-      <c r="D91" s="1"/>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="D91" s="5">
+        <v>44128</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -1891,11 +1917,14 @@
         <v>2</v>
       </c>
       <c r="C92" s="2">
-        <v>0</v>
-      </c>
-      <c r="D92" s="1"/>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="D92" s="5">
+        <v>44129</v>
+      </c>
+      <c r="G92" s="6"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -1907,7 +1936,7 @@
       </c>
       <c r="D93" s="1"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -1919,7 +1948,7 @@
       </c>
       <c r="D94" s="1"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -1931,7 +1960,7 @@
       </c>
       <c r="D95" s="1"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>94</v>
       </c>

</xml_diff>